<commit_message>
Doc update (Planen & Entscheiden) Klassendiagram + Aktivitätsdiagram
</commit_message>
<xml_diff>
--- a/Doc/Gantt.xlsx
+++ b/Doc/Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsordner\_ImportantStuff\Torben_Dziuk_stuff\2teProbeIPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeitsordner\_ImportantStuff\Torben_Dziuk_stuff\2teProbeIPA\ProbeIPATorben\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D1255456-B8C8-4A53-9DB8-4A1634435D93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{75FEC8C0-1CC6-450C-A11E-9C4CBB087A0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{7368EEC8-37A3-4D19-88FF-F7E147FC3DC2}"/>
   </bookViews>
@@ -915,7 +915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1037,81 +1037,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1269,21 +1194,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1318,6 +1228,108 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1636,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D6F5E9-624B-4CCE-882E-0793EA18CA51}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,72 +1658,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="116"/>
+      <c r="C1" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="52" t="s">
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="52" t="s">
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="52" t="s">
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="52" t="s">
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="109"/>
+      <c r="T1" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="121"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="109"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="123"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="123"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="122"/>
-      <c r="U2" s="123"/>
-      <c r="V2" s="123"/>
-      <c r="W2" s="124"/>
+      <c r="A2" s="116"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="112"/>
     </row>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="117"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
@@ -1772,1253 +1784,1255 @@
       <c r="V3" s="19">
         <v>6</v>
       </c>
-      <c r="W3" s="125">
+      <c r="W3" s="95">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="114" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="106"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="81"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="67"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="67"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="98"/>
-      <c r="W4" s="126"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="96"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="134"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
       <c r="F5" s="39"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="70"/>
+      <c r="K5" s="45"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="70"/>
+      <c r="O5" s="45"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="82"/>
+      <c r="S5" s="57"/>
       <c r="T5" s="4"/>
       <c r="U5" s="5"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="127"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="97"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="61" t="s">
+      <c r="A6" s="134"/>
+      <c r="B6" s="113" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="107"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="70"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="4"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="70"/>
+      <c r="O6" s="45"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="82"/>
+      <c r="S6" s="57"/>
       <c r="T6" s="4"/>
       <c r="U6" s="5"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="127"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="97"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="61"/>
+      <c r="A7" s="134"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="39"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="70"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="4"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="70"/>
+      <c r="O7" s="45"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="82"/>
+      <c r="S7" s="57"/>
       <c r="T7" s="4"/>
       <c r="U7" s="5"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="127"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="97"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="134"/>
+      <c r="B8" s="113" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="86"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="108"/>
+      <c r="H8" s="83"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="70"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="4"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="70"/>
+      <c r="O8" s="45"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="82"/>
+      <c r="S8" s="57"/>
       <c r="T8" s="4"/>
       <c r="U8" s="5"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="127"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="97"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="86"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="137"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="70"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="70"/>
+      <c r="O9" s="45"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="82"/>
+      <c r="S9" s="57"/>
       <c r="T9" s="4"/>
       <c r="U9" s="5"/>
-      <c r="V9" s="99"/>
-      <c r="W9" s="127"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="97"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="61" t="s">
+      <c r="A10" s="134"/>
+      <c r="B10" s="113" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="86"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="108"/>
+      <c r="H10" s="83"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="70"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="4"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="70"/>
+      <c r="O10" s="45"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="82"/>
+      <c r="S10" s="57"/>
       <c r="T10" s="4"/>
       <c r="U10" s="5"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="127"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="97"/>
     </row>
     <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="85"/>
-      <c r="E11" s="86"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="137"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="70"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="4"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="70"/>
+      <c r="O11" s="45"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="82"/>
+      <c r="S11" s="57"/>
       <c r="T11" s="4"/>
       <c r="U11" s="5"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="127"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="97"/>
     </row>
     <row r="12" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="125" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="87"/>
-      <c r="E12" s="88"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="63"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="111"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="86"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="77"/>
+      <c r="K12" s="52"/>
       <c r="L12" s="6"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="77"/>
+      <c r="O12" s="52"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="77"/>
+      <c r="S12" s="52"/>
       <c r="T12" s="6"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="100"/>
-      <c r="W12" s="128"/>
+      <c r="V12" s="75"/>
+      <c r="W12" s="98"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="128"/>
+      <c r="B13" s="129"/>
       <c r="C13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="89"/>
-      <c r="E13" s="86"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="70"/>
+      <c r="K13" s="45"/>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="70"/>
+      <c r="O13" s="45"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="70"/>
+      <c r="S13" s="45"/>
       <c r="T13" s="2"/>
       <c r="U13" s="3"/>
-      <c r="V13" s="101"/>
-      <c r="W13" s="129"/>
+      <c r="V13" s="76"/>
+      <c r="W13" s="99"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="41" t="s">
+      <c r="A14" s="128"/>
+      <c r="B14" s="115" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="69"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="107"/>
+      <c r="I14" s="82"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="70"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="70"/>
+      <c r="O14" s="45"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="70"/>
+      <c r="S14" s="45"/>
       <c r="T14" s="2"/>
       <c r="U14" s="3"/>
-      <c r="V14" s="101"/>
-      <c r="W14" s="129"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="99"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="128"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="86"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="70"/>
+      <c r="K15" s="45"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="70"/>
+      <c r="O15" s="45"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="70"/>
+      <c r="S15" s="45"/>
       <c r="T15" s="2"/>
       <c r="U15" s="3"/>
-      <c r="V15" s="101"/>
-      <c r="W15" s="129"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="99"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="44"/>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="128"/>
+      <c r="B16" s="115" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="107"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="82"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="70"/>
+      <c r="K16" s="45"/>
       <c r="L16" s="2"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="70"/>
+      <c r="O16" s="45"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="70"/>
+      <c r="S16" s="45"/>
       <c r="T16" s="2"/>
       <c r="U16" s="3"/>
-      <c r="V16" s="101"/>
-      <c r="W16" s="129"/>
+      <c r="V16" s="76"/>
+      <c r="W16" s="99"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" s="44"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="86"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="70"/>
+      <c r="K17" s="45"/>
       <c r="L17" s="2"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="70"/>
+      <c r="O17" s="45"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="70"/>
+      <c r="S17" s="45"/>
       <c r="T17" s="2"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="101"/>
-      <c r="W17" s="129"/>
+      <c r="V17" s="76"/>
+      <c r="W17" s="99"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
-      <c r="B18" s="41" t="s">
+      <c r="A18" s="128"/>
+      <c r="B18" s="115" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="86"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="107"/>
-      <c r="K18" s="70"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="45"/>
       <c r="L18" s="2"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="70"/>
+      <c r="O18" s="45"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="70"/>
+      <c r="S18" s="45"/>
       <c r="T18" s="2"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="101"/>
-      <c r="W18" s="129"/>
+      <c r="V18" s="76"/>
+      <c r="W18" s="99"/>
     </row>
     <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="132"/>
+      <c r="B19" s="135"/>
       <c r="C19" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="94"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="74"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="104"/>
-      <c r="W19" s="130"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="54"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="79"/>
+      <c r="W19" s="100"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="126" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="92"/>
-      <c r="E20" s="93"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="10"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="110"/>
-      <c r="K20" s="119"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="94"/>
       <c r="L20" s="10"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="72"/>
+      <c r="O20" s="47"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
-      <c r="S20" s="72"/>
+      <c r="S20" s="47"/>
       <c r="T20" s="10"/>
       <c r="U20" s="9"/>
-      <c r="V20" s="103"/>
-      <c r="W20" s="131"/>
+      <c r="V20" s="78"/>
+      <c r="W20" s="101"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="128"/>
+      <c r="B21" s="129"/>
       <c r="C21" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="92"/>
-      <c r="E21" s="93"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="68"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="10"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="72"/>
+      <c r="J21" s="139"/>
+      <c r="K21" s="47"/>
       <c r="L21" s="10"/>
       <c r="M21" s="3"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="72"/>
+      <c r="O21" s="47"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
-      <c r="S21" s="72"/>
+      <c r="S21" s="47"/>
       <c r="T21" s="10"/>
       <c r="U21" s="9"/>
-      <c r="V21" s="103"/>
-      <c r="W21" s="131"/>
+      <c r="V21" s="78"/>
+      <c r="W21" s="101"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="128"/>
+      <c r="B22" s="115" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="92"/>
-      <c r="E22" s="93"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="68"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="10"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="113"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="88"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="66"/>
+      <c r="M22" s="41"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="72"/>
+      <c r="O22" s="47"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
-      <c r="S22" s="72"/>
+      <c r="S22" s="47"/>
       <c r="T22" s="10"/>
       <c r="U22" s="9"/>
-      <c r="V22" s="103"/>
-      <c r="W22" s="131"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="101"/>
     </row>
     <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="44"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="128"/>
+      <c r="B23" s="129"/>
       <c r="C23" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="92"/>
-      <c r="E23" s="93"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="72"/>
+      <c r="J23" s="139"/>
+      <c r="K23" s="47"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="73"/>
+      <c r="M23" s="48"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="72"/>
+      <c r="O23" s="47"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="72"/>
+      <c r="S23" s="47"/>
       <c r="T23" s="10"/>
       <c r="U23" s="9"/>
-      <c r="V23" s="103"/>
-      <c r="W23" s="131"/>
+      <c r="V23" s="78"/>
+      <c r="W23" s="101"/>
     </row>
     <row r="24" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="125" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="87"/>
-      <c r="E24" s="88"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="63"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="114"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="89"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="77"/>
+      <c r="O24" s="52"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="77"/>
+      <c r="S24" s="52"/>
       <c r="T24" s="6"/>
       <c r="U24" s="1"/>
-      <c r="V24" s="100"/>
-      <c r="W24" s="128"/>
+      <c r="V24" s="75"/>
+      <c r="W24" s="98"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="129"/>
       <c r="C25" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="E25" s="86"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="61"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="70"/>
+      <c r="K25" s="45"/>
       <c r="L25" s="2"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="70"/>
+      <c r="O25" s="45"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="70"/>
+      <c r="S25" s="45"/>
       <c r="T25" s="2"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="101"/>
-      <c r="W25" s="129"/>
+      <c r="V25" s="76"/>
+      <c r="W25" s="99"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A26" s="44"/>
-      <c r="B26" s="41" t="s">
+      <c r="A26" s="128"/>
+      <c r="B26" s="115" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="89"/>
-      <c r="E26" s="86"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="61"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="115"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="90"/>
       <c r="M26" s="16"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="72"/>
+      <c r="O26" s="47"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="70"/>
+      <c r="S26" s="45"/>
       <c r="T26" s="2"/>
       <c r="U26" s="3"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="129"/>
+      <c r="V26" s="76"/>
+      <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
-      <c r="B27" s="46"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="126"/>
       <c r="C27" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="86"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="61"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="70"/>
+      <c r="K27" s="45"/>
       <c r="L27" s="2"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="70"/>
+      <c r="O27" s="45"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="70"/>
+      <c r="S27" s="45"/>
       <c r="T27" s="2"/>
       <c r="U27" s="3"/>
-      <c r="V27" s="101"/>
-      <c r="W27" s="129"/>
+      <c r="V27" s="76"/>
+      <c r="W27" s="99"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A28" s="44"/>
-      <c r="B28" s="41" t="s">
+      <c r="A28" s="128"/>
+      <c r="B28" s="115" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="86"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="61"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="70"/>
+      <c r="K28" s="45"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="116"/>
-      <c r="P28" s="115"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="91"/>
+      <c r="P28" s="90"/>
       <c r="Q28" s="16"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="70"/>
+      <c r="S28" s="45"/>
       <c r="T28" s="2"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="101"/>
-      <c r="W28" s="129"/>
+      <c r="V28" s="76"/>
+      <c r="W28" s="99"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A29" s="44"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="128"/>
+      <c r="B29" s="129"/>
       <c r="C29" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="89"/>
-      <c r="E29" s="86"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="61"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="70"/>
+      <c r="K29" s="45"/>
       <c r="L29" s="2"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="70"/>
+      <c r="O29" s="45"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="70"/>
+      <c r="S29" s="45"/>
       <c r="T29" s="2"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="101"/>
-      <c r="W29" s="129"/>
+      <c r="V29" s="76"/>
+      <c r="W29" s="99"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A30" s="44"/>
-      <c r="B30" s="41" t="s">
+      <c r="A30" s="128"/>
+      <c r="B30" s="115" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="89"/>
-      <c r="E30" s="86"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="61"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="70"/>
+      <c r="K30" s="45"/>
       <c r="L30" s="2"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="70"/>
-      <c r="P30" s="115"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="82"/>
       <c r="S30" s="34"/>
       <c r="T30" s="2"/>
       <c r="U30" s="3"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="129"/>
+      <c r="V30" s="76"/>
+      <c r="W30" s="99"/>
     </row>
     <row r="31" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="44"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="128"/>
+      <c r="B31" s="129"/>
       <c r="C31" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="89"/>
-      <c r="E31" s="86"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="61"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="70"/>
+      <c r="K31" s="45"/>
       <c r="L31" s="2"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="70"/>
+      <c r="O31" s="45"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="70"/>
+      <c r="S31" s="45"/>
       <c r="T31" s="2"/>
       <c r="U31" s="3"/>
-      <c r="V31" s="101"/>
-      <c r="W31" s="129"/>
+      <c r="V31" s="76"/>
+      <c r="W31" s="99"/>
     </row>
     <row r="32" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="125" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="87"/>
-      <c r="E32" s="88"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="6"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="77"/>
+      <c r="K32" s="52"/>
       <c r="L32" s="6"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="77"/>
+      <c r="O32" s="52"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="117"/>
+      <c r="S32" s="92"/>
       <c r="T32" s="6"/>
       <c r="U32" s="1"/>
-      <c r="V32" s="100"/>
-      <c r="W32" s="128"/>
+      <c r="V32" s="75"/>
+      <c r="W32" s="98"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A33" s="44"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="128"/>
+      <c r="B33" s="129"/>
       <c r="C33" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="89"/>
-      <c r="E33" s="86"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="61"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="2"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="70"/>
+      <c r="K33" s="45"/>
       <c r="L33" s="2"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="70"/>
+      <c r="O33" s="45"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="34"/>
       <c r="T33" s="2"/>
       <c r="U33" s="3"/>
-      <c r="V33" s="101"/>
-      <c r="W33" s="129"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="99"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
-      <c r="B34" s="41" t="s">
+      <c r="A34" s="128"/>
+      <c r="B34" s="115" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="89"/>
-      <c r="E34" s="86"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="61"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="2"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="70"/>
+      <c r="K34" s="45"/>
       <c r="L34" s="2"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="70"/>
+      <c r="O34" s="45"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="116"/>
+      <c r="S34" s="91"/>
       <c r="T34" s="2"/>
       <c r="U34" s="3"/>
-      <c r="V34" s="101"/>
-      <c r="W34" s="129"/>
+      <c r="V34" s="76"/>
+      <c r="W34" s="99"/>
     </row>
     <row r="35" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="48"/>
-      <c r="B35" s="57"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="66"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
-      <c r="K35" s="78"/>
+      <c r="K35" s="53"/>
       <c r="L35" s="8"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
-      <c r="O35" s="78"/>
+      <c r="O35" s="53"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
-      <c r="S35" s="78"/>
+      <c r="S35" s="53"/>
       <c r="T35" s="8"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="102"/>
-      <c r="W35" s="132"/>
+      <c r="V35" s="77"/>
+      <c r="W35" s="102"/>
     </row>
     <row r="36" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="125" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="87"/>
-      <c r="E36" s="88"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="63"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="6"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="77"/>
+      <c r="K36" s="52"/>
       <c r="L36" s="6"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
-      <c r="O36" s="77"/>
+      <c r="O36" s="52"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="77"/>
-      <c r="T36" s="114"/>
+      <c r="S36" s="52"/>
+      <c r="T36" s="89"/>
       <c r="U36" s="1"/>
-      <c r="V36" s="100"/>
-      <c r="W36" s="128"/>
+      <c r="V36" s="75"/>
+      <c r="W36" s="98"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
-      <c r="B37" s="46"/>
+      <c r="A37" s="128"/>
+      <c r="B37" s="126"/>
       <c r="C37" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="89"/>
-      <c r="E37" s="86"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="61"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="2"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="70"/>
+      <c r="K37" s="45"/>
       <c r="L37" s="2"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="70"/>
+      <c r="O37" s="45"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="70"/>
+      <c r="S37" s="45"/>
       <c r="T37" s="2"/>
       <c r="U37" s="3"/>
-      <c r="V37" s="101"/>
-      <c r="W37" s="129"/>
+      <c r="V37" s="76"/>
+      <c r="W37" s="99"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" s="44"/>
-      <c r="B38" s="41" t="s">
+      <c r="A38" s="128"/>
+      <c r="B38" s="115" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="89"/>
-      <c r="E38" s="86"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="2"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="70"/>
+      <c r="K38" s="45"/>
       <c r="L38" s="2"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="70"/>
+      <c r="O38" s="45"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="70"/>
-      <c r="T38" s="115"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="90"/>
       <c r="U38" s="3"/>
-      <c r="V38" s="101"/>
-      <c r="W38" s="129"/>
+      <c r="V38" s="76"/>
+      <c r="W38" s="99"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" s="44"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="128"/>
+      <c r="B39" s="129"/>
       <c r="C39" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="89"/>
-      <c r="E39" s="86"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="2"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
-      <c r="K39" s="70"/>
+      <c r="K39" s="45"/>
       <c r="L39" s="2"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="70"/>
+      <c r="O39" s="45"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="70"/>
+      <c r="S39" s="45"/>
       <c r="T39" s="2"/>
       <c r="U39" s="3"/>
-      <c r="V39" s="101"/>
-      <c r="W39" s="129"/>
+      <c r="V39" s="76"/>
+      <c r="W39" s="99"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="44"/>
-      <c r="B40" s="41" t="s">
+      <c r="A40" s="128"/>
+      <c r="B40" s="115" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="89"/>
-      <c r="E40" s="86"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="61"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="2"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="70"/>
+      <c r="K40" s="45"/>
       <c r="L40" s="2"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="70"/>
+      <c r="O40" s="45"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="70"/>
+      <c r="S40" s="45"/>
       <c r="T40" s="2"/>
-      <c r="U40" s="107"/>
-      <c r="V40" s="101"/>
-      <c r="W40" s="129"/>
+      <c r="U40" s="82"/>
+      <c r="V40" s="76"/>
+      <c r="W40" s="99"/>
     </row>
     <row r="41" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="45"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="132"/>
+      <c r="B41" s="135"/>
       <c r="C41" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="94"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="73"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="74"/>
-      <c r="M41" s="73"/>
-      <c r="N41" s="73"/>
-      <c r="O41" s="79"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="73"/>
-      <c r="R41" s="73"/>
-      <c r="S41" s="79"/>
-      <c r="T41" s="74"/>
-      <c r="U41" s="73"/>
-      <c r="V41" s="104"/>
-      <c r="W41" s="130"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="54"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="48"/>
+      <c r="R41" s="48"/>
+      <c r="S41" s="54"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="48"/>
+      <c r="V41" s="79"/>
+      <c r="W41" s="100"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" s="44"/>
-      <c r="B42" s="49" t="s">
+      <c r="A42" s="128"/>
+      <c r="B42" s="136" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="96"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="109"/>
-      <c r="H42" s="75"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="80"/>
-      <c r="L42" s="75"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76"/>
-      <c r="O42" s="80"/>
-      <c r="P42" s="75"/>
-      <c r="Q42" s="76"/>
-      <c r="R42" s="76"/>
-      <c r="S42" s="80"/>
-      <c r="T42" s="75"/>
-      <c r="U42" s="76"/>
-      <c r="V42" s="105"/>
-      <c r="W42" s="133"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="55"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="80"/>
+      <c r="W42" s="103"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A43" s="44"/>
-      <c r="B43" s="42"/>
+      <c r="A43" s="128"/>
+      <c r="B43" s="129"/>
       <c r="C43" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="89"/>
-      <c r="E43" s="86"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="61"/>
       <c r="F43" s="3"/>
       <c r="G43" s="39"/>
       <c r="H43" s="2"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
-      <c r="K43" s="70"/>
+      <c r="K43" s="45"/>
       <c r="L43" s="2"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="70"/>
+      <c r="O43" s="45"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
-      <c r="S43" s="70"/>
+      <c r="S43" s="45"/>
       <c r="T43" s="2"/>
       <c r="U43" s="3"/>
-      <c r="V43" s="101"/>
-      <c r="W43" s="129"/>
+      <c r="V43" s="76"/>
+      <c r="W43" s="99"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A44" s="44"/>
-      <c r="B44" s="46" t="s">
+      <c r="A44" s="128"/>
+      <c r="B44" s="126" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="92"/>
-      <c r="E44" s="93"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="68"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="110"/>
+      <c r="G44" s="85"/>
       <c r="H44" s="10"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
-      <c r="K44" s="112"/>
+      <c r="K44" s="87"/>
       <c r="L44" s="10"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
-      <c r="O44" s="112"/>
+      <c r="O44" s="87"/>
       <c r="P44" s="10"/>
       <c r="Q44" s="9"/>
       <c r="R44" s="9"/>
-      <c r="S44" s="112"/>
+      <c r="S44" s="87"/>
       <c r="T44" s="10"/>
-      <c r="U44" s="110"/>
-      <c r="V44" s="103"/>
-      <c r="W44" s="131"/>
+      <c r="U44" s="85"/>
+      <c r="V44" s="78"/>
+      <c r="W44" s="101"/>
     </row>
     <row r="45" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="48"/>
-      <c r="B45" s="42"/>
+      <c r="A45" s="130"/>
+      <c r="B45" s="129"/>
       <c r="C45" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="94"/>
-      <c r="E45" s="95"/>
-      <c r="F45" s="73"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="48"/>
       <c r="G45" s="40"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="73"/>
-      <c r="O45" s="79"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="73"/>
-      <c r="S45" s="79"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="73"/>
-      <c r="V45" s="104"/>
-      <c r="W45" s="130"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="140"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="54"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="48"/>
+      <c r="S45" s="54"/>
+      <c r="T45" s="49"/>
+      <c r="U45" s="48"/>
+      <c r="V45" s="79"/>
+      <c r="W45" s="100"/>
     </row>
     <row r="46" spans="1:23" ht="67.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50" t="s">
+      <c r="A46" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="134" t="s">
+      <c r="B46" s="124"/>
+      <c r="C46" s="124"/>
+      <c r="D46" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="134"/>
-      <c r="F46" s="134"/>
-      <c r="G46" s="134"/>
-      <c r="H46" s="134" t="s">
+      <c r="E46" s="104"/>
+      <c r="F46" s="104"/>
+      <c r="G46" s="104"/>
+      <c r="H46" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="I46" s="134"/>
-      <c r="J46" s="134" t="s">
+      <c r="I46" s="104"/>
+      <c r="J46" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="K46" s="134" t="s">
+      <c r="K46" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="L46" s="134"/>
-      <c r="M46" s="135"/>
-      <c r="N46" s="134"/>
-      <c r="O46" s="134"/>
-      <c r="P46" s="134"/>
-      <c r="Q46" s="136"/>
-      <c r="R46" s="134" t="s">
+      <c r="L46" s="104"/>
+      <c r="M46" s="105"/>
+      <c r="N46" s="104"/>
+      <c r="O46" s="104"/>
+      <c r="P46" s="104"/>
+      <c r="Q46" s="106"/>
+      <c r="R46" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="S46" s="134" t="s">
+      <c r="S46" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="T46" s="134"/>
-      <c r="U46" s="134" t="s">
+      <c r="T46" s="104"/>
+      <c r="U46" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="V46" s="134" t="s">
+      <c r="V46" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="W46" s="134"/>
+      <c r="W46" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="L1:O2"/>
-    <mergeCell ref="P1:S2"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="T1:W2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="A24:A31"/>
@@ -3026,13 +3040,6 @@
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B18:B19"/>
     <mergeCell ref="A36:A41"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B44:B45"/>
@@ -3040,11 +3047,16 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="T1:W2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="L1:O2"/>
+    <mergeCell ref="P1:S2"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>